<commit_message>
Add spreadsheet for API Spreadsheet
</commit_message>
<xml_diff>
--- a/data/contact-form.xlsx
+++ b/data/contact-form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taliha/Programming/GitHub/my-projects/spellbinding-website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taliha/Programming/GitHub/my-projects/spellbinding-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1546A926-3500-C441-9BBA-98DB4E719D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5783DA2-479F-1549-991C-E1521D1F8716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="1460" windowWidth="28040" windowHeight="16020" xr2:uid="{600229DB-AD56-A648-98D8-A81F3CFB107C}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{600229DB-AD56-A648-98D8-A81F3CFB107C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>user_name</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>user_msg</t>
-  </si>
-  <si>
-    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -91,9 +88,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,25 +406,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF60009-796B-F346-973F-138725178A35}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>